<commit_message>
update the map with time
</commit_message>
<xml_diff>
--- a/Simulator/lib.xlsx
+++ b/Simulator/lib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baizishan/Documents/Library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\OneDrive - UW-Madison\Desktop\New Dream\Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{389BE363-5D0E-6C44-AE6B-4CE00BACF833}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AB98C4-75C8-4606-AB44-981DBDD8F65B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16220" xr2:uid="{D9B3C0E5-8B68-E249-8A49-1ED7C8FA4432}"/>
+    <workbookView xWindow="12615" yWindow="2760" windowWidth="21600" windowHeight="11595" xr2:uid="{D9B3C0E5-8B68-E249-8A49-1ED7C8FA4432}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,48 +30,57 @@
     <t>Library</t>
   </si>
   <si>
-    <t>Ashman</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
-    <t>Hawthorne</t>
-  </si>
-  <si>
-    <t>Lakeview</t>
-  </si>
-  <si>
-    <t>Meadowridge</t>
-  </si>
-  <si>
-    <t>Monroe Street</t>
-  </si>
-  <si>
-    <t>Pinney</t>
-  </si>
-  <si>
-    <t>Sequoya</t>
-  </si>
-  <si>
-    <t>South Madison</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>SEQ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -80,6 +89,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,7 +123,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,7 +139,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -422,28 +438,28 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>43.076070999999999</v>
@@ -452,9 +468,9 @@
         <v>-89.517674</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>43.073690999999997</v>
@@ -463,9 +479,9 @@
         <v>-89.387406999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>43.101474000000003</v>
@@ -474,9 +490,9 @@
         <v>-89.346345999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>43.127783000000001</v>
@@ -485,7 +501,7 @@
         <v>-89.362314999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -496,9 +512,9 @@
         <v>-89.479142999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>43.065924000000003</v>
@@ -507,9 +523,9 @@
         <v>-89.415187000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>43.084485999999998</v>
@@ -518,9 +534,9 @@
         <v>-89.323933999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
         <v>43.053815999999998</v>
@@ -529,9 +545,9 @@
         <v>-89.450558000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>43.04128</v>
@@ -541,6 +557,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>